<commit_message>
Cambiar verificación del nombre de plantillas
Co-Authored-By: Juan Diego <68799845+juandiego-gm@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple (19).xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple (19).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF03C39A-186C-6449-B6D0-1C055FD0A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE4FFFF-EDA3-0741-BFE8-A27F5352E194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36240" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,124 +20,133 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
-  <si>
-    <t>LUNES, 01/07/2024</t>
-  </si>
-  <si>
-    <t>MARTES, 02/07/2024</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 03/07/2024</t>
-  </si>
-  <si>
-    <t>JUEVES, 04/07/2024</t>
-  </si>
-  <si>
-    <t>VIERNES, 05/07/2024</t>
-  </si>
-  <si>
-    <t>SÁBADO, 06/07/2024</t>
-  </si>
-  <si>
-    <t>DOMINGO, 07/07/2024</t>
-  </si>
-  <si>
-    <t>LUNES, 08/07/2024</t>
-  </si>
-  <si>
-    <t>MARTES, 09/07/2024</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 10/07/2024</t>
-  </si>
-  <si>
-    <t>JUEVES, 11/07/2024</t>
-  </si>
-  <si>
-    <t>VIERNES, 12/07/2024</t>
-  </si>
-  <si>
-    <t>SÁBADO, 13/07/2024</t>
-  </si>
-  <si>
-    <t>DOMINGO, 14/07/2024</t>
-  </si>
-  <si>
-    <t>LUNES, 15/07/2024</t>
-  </si>
-  <si>
-    <t>MARTES, 16/07/2024</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 17/07/2024</t>
-  </si>
-  <si>
-    <t>JUEVES, 18/07/2024</t>
-  </si>
-  <si>
-    <t>VIERNES, 19/07/2024</t>
-  </si>
-  <si>
-    <t>SÁBADO, 20/07/2024</t>
-  </si>
-  <si>
-    <t>DOMINGO, 21/07/2024</t>
-  </si>
-  <si>
-    <t>LUNES, 22/07/2024</t>
-  </si>
-  <si>
-    <t>MARTES, 23/07/2024</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 24/07/2024</t>
-  </si>
-  <si>
-    <t>JUEVES, 25/07/2024</t>
-  </si>
-  <si>
-    <t>VIERNES, 26/07/2024</t>
-  </si>
-  <si>
-    <t>SÁBADO, 27/07/2024</t>
-  </si>
-  <si>
-    <t>DOMINGO, 28/07/2024</t>
-  </si>
-  <si>
-    <t>LUNES, 29/07/2024</t>
-  </si>
-  <si>
-    <t>MARTES, 30/07/2024</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 31/07/2024</t>
-  </si>
-  <si>
-    <t>1851841891</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="36">
+  <si>
+    <t>EMPLEADO</t>
+  </si>
+  <si>
+    <t>JUEVES, 01/08/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 02/08/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 03/08/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 04/08/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 05/08/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 06/08/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 07/08/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 08/08/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 09/08/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 10/08/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 11/08/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 12/08/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 13/08/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 14/08/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 15/08/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 16/08/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 17/08/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 18/08/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 19/08/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 20/08/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 21/08/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 22/08/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 23/08/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 24/08/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 25/08/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 26/08/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 27/08/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 28/08/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 29/08/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 30/08/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 31/08/2024</t>
+  </si>
+  <si>
+    <t>1722128905</t>
   </si>
   <si>
     <t>1759787615</t>
   </si>
   <si>
+    <t>1759787616</t>
+  </si>
+  <si>
     <t>OFICINA</t>
-  </si>
-  <si>
-    <t>EMPLEADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,146 +524,400 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:AF1 A3 A2 G2:AF2 G3:AF3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:AF1 A3:A4 A2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-	Colocar en la plantilla el apellido y nombre del usuario.
Co-Authored-By: Juan Diego <68799845+juandiego-gm@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple (19).xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple (19).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE4FFFF-EDA3-0741-BFE8-A27F5352E194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0FAA5B-192B-7140-B73E-944BF7671A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
   <si>
     <t>EMPLEADO</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>OFICINA</t>
+  </si>
+  <si>
+    <t>OFICINA,DEFAULT-LIBRE</t>
+  </si>
+  <si>
+    <t>1758796831</t>
   </si>
 </sst>
 </file>
@@ -169,9 +175,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,7 +736,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>35</v>
@@ -912,6 +919,11 @@
       </c>
       <c r="AF4" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>